<commit_message>
Excel sheet updated with 5,6,7,8,9 node times
</commit_message>
<xml_diff>
--- a/Lab3/src/lab3.xlsx
+++ b/Lab3/src/lab3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/reidaruss/Desktop/Junior_Year/Algorithms/Reid_Russell_CS3353/Lab3/src/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5524DBF-A829-0047-BE52-B8A696951CC7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344CCBC5-8F36-C746-9DFE-B49463A0CF8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18320" yWindow="1960" windowWidth="16640" windowHeight="17440" xr2:uid="{F87358E0-4A70-144F-A56E-8728BB4DCB34}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Brute Force Runtimes</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Time (s)</t>
+  </si>
+  <si>
+    <t>Dynamic Programming Runtimes</t>
   </si>
 </sst>
 </file>
@@ -392,18 +395,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBF5B89A-D687-6046-9EC7-D921DE238BB0}">
-  <dimension ref="C4:E9"/>
+  <dimension ref="C4:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="7" max="7" width="27.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -413,45 +417,175 @@
       <c r="E4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D5">
         <v>4</v>
       </c>
       <c r="E5" s="1">
         <v>4.1548999999999998E-5</v>
       </c>
-    </row>
-    <row r="6" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="H5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D6">
+        <v>5</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.0498099999999999E-4</v>
+      </c>
+      <c r="H6">
+        <f>H5+1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="1">
+        <v>6.1086400000000003E-4</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ref="H7:H21" si="0">H6+1</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3.6273899999999999E-3</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3.5053000000000001E-2</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.36330299999999999</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D11">
         <v>10</v>
       </c>
-      <c r="E6">
+      <c r="E11">
         <v>2.9923199999999999</v>
       </c>
-    </row>
-    <row r="7" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D7">
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D12">
         <v>11</v>
       </c>
-      <c r="E7">
+      <c r="E12">
         <v>28.286899999999999</v>
       </c>
-    </row>
-    <row r="8" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D8">
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D13">
         <v>12</v>
       </c>
-      <c r="E8">
+      <c r="E13">
         <v>339.44799999999998</v>
       </c>
-    </row>
-    <row r="9" spans="3:5" x14ac:dyDescent="0.2">
-      <c r="D9">
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D14">
         <v>13</v>
       </c>
-      <c r="E9">
+      <c r="E14">
         <v>4850.46</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H18">
+        <f>H17+1</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="8:8" x14ac:dyDescent="0.2">
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>